<commit_message>
feat: add scenario field and rename Suite to Submodule terminology
Phase 1 (Completed):
- Add scenario field to TestCase entity and DTO
- Rename TestSuite to TestSubmodule throughout codebase
- Update database tables, entities, repositories, DTOs
- Update API endpoints from /testsuites to /testsubmodules
- Update Excel template: Suite Name → Submodule Name, add Scenario column
- Update frontend models, services, and components
- Update UI labels and references

Phase 2 (Completed):
- Create domain service classes (ProjectService, ModuleService, SubmoduleService, TestCaseService, ExecutionService)
- Add domain service dependencies to TcmService and ApiController
- Refactor TcmService to delegate to domain services

Database changes:
- test_suites → test_submodules table
- test_cases table: add scenario column, update submodule references
- Uses ddl-auto=create for automatic schema creation
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/test-case-import-template.xlsx
+++ b/src/main/resources/templates/test-case-import-template.xlsx
@@ -452,7 +452,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -470,37 +470,42 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Suite Name</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Submodule Name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
         <is>
           <t>Test Case ID</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>Title</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>Description</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Scenario</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
         <is>
           <t>Step Number</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>Action</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>Expected Result</t>
         </is>

</xml_diff>

<commit_message>
docs: update excel import template
- Regenerated Excel import template to align with current terminology and import logic.

- Removed unused Scenario column from the template.

- Updated instructions to use Submodule Name instead of Suite Name.

- Added grouping pattern explanation in instructions.

- Updated sample data to be more representative of real test scenarios.

- The template now correctly matches the ImportExportService expectations.
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/test-case-import-template.xlsx
+++ b/src/main/resources/templates/test-case-import-template.xlsx
@@ -38,7 +38,7 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
@@ -51,8 +51,14 @@
         <bgColor rgb="004472C4"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00D9E1F2"/>
+        <bgColor rgb="00D9E1F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -60,33 +66,17 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -452,340 +442,336 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="22.8" customWidth="1" min="1" max="1"/>
-    <col width="16.8" customWidth="1" min="2" max="2"/>
-    <col width="36" customWidth="1" min="3" max="3"/>
-    <col width="33.6" customWidth="1" min="4" max="4"/>
-    <col width="15.6" customWidth="1" min="5" max="5"/>
-    <col width="49.2" customWidth="1" min="6" max="6"/>
-    <col width="49.2" customWidth="1" min="7" max="7"/>
+    <col width="25" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="40" customWidth="1" min="3" max="3"/>
+    <col width="40" customWidth="1" min="4" max="4"/>
+    <col width="12" customWidth="1" min="5" max="5"/>
+    <col width="40" customWidth="1" min="6" max="6"/>
+    <col width="40" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Submodule Name</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Test Case ID</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Title</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Description</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Scenario</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Step Number</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Action</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Expected Result</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="inlineStr">
-        <is>
-          <t>User Login</t>
-        </is>
-      </c>
-      <c r="B2" s="2" t="inlineStr">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>User Authentication</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
         <is>
           <t>TC-001</t>
         </is>
       </c>
-      <c r="C2" s="2" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>Login with valid credentials</t>
         </is>
       </c>
-      <c r="D2" s="2" t="inlineStr">
-        <is>
-          <t>Test successful login flow</t>
-        </is>
-      </c>
-      <c r="E2" s="2" t="n">
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Test successful login flow with correct username and password</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
         <v>1</v>
       </c>
-      <c r="F2" s="2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>Navigate to login page</t>
         </is>
       </c>
-      <c r="G2" s="2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>Login form is displayed</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="inlineStr">
-        <is>
-          <t>User Login</t>
-        </is>
-      </c>
-      <c r="B3" s="2" t="inlineStr">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>User Authentication</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
         <is>
           <t>TC-001</t>
         </is>
       </c>
-      <c r="C3" s="2" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>Login with valid credentials</t>
         </is>
       </c>
-      <c r="D3" s="2" t="inlineStr">
-        <is>
-          <t>Test successful login flow</t>
-        </is>
-      </c>
-      <c r="E3" s="2" t="n">
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Test successful login flow with correct username and password</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
         <v>2</v>
       </c>
-      <c r="F3" s="2" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>Enter valid username and password</t>
         </is>
       </c>
-      <c r="G3" s="2" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>Credentials are accepted</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>User Login</t>
-        </is>
-      </c>
-      <c r="B4" s="2" t="inlineStr">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>User Authentication</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
         <is>
           <t>TC-001</t>
         </is>
       </c>
-      <c r="C4" s="2" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>Login with valid credentials</t>
         </is>
       </c>
-      <c r="D4" s="2" t="inlineStr">
-        <is>
-          <t>Test successful login flow</t>
-        </is>
-      </c>
-      <c r="E4" s="2" t="n">
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Test successful login flow with correct username and password</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
         <v>3</v>
       </c>
-      <c r="F4" s="2" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>Click Login button</t>
         </is>
       </c>
-      <c r="G4" s="2" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>User is redirected to dashboard</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="inlineStr">
-        <is>
-          <t>User Login</t>
-        </is>
-      </c>
-      <c r="B5" s="2" t="inlineStr">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>User Authentication</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
         <is>
           <t>TC-002</t>
         </is>
       </c>
-      <c r="C5" s="2" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>Login with invalid password</t>
         </is>
       </c>
-      <c r="D5" s="2" t="inlineStr">
-        <is>
-          <t>Test password validation</t>
-        </is>
-      </c>
-      <c r="E5" s="2" t="n">
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Test password validation when incorrect password is provided</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
         <v>1</v>
       </c>
-      <c r="F5" s="2" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>Navigate to login page</t>
         </is>
       </c>
-      <c r="G5" s="2" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>Login form is displayed</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="inlineStr">
-        <is>
-          <t>User Login</t>
-        </is>
-      </c>
-      <c r="B6" s="2" t="inlineStr">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>User Authentication</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
         <is>
           <t>TC-002</t>
         </is>
       </c>
-      <c r="C6" s="2" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>Login with invalid password</t>
         </is>
       </c>
-      <c r="D6" s="2" t="inlineStr">
-        <is>
-          <t>Test password validation</t>
-        </is>
-      </c>
-      <c r="E6" s="2" t="n">
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Test password validation when incorrect password is provided</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
         <v>2</v>
       </c>
-      <c r="F6" s="2" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>Enter valid username and wrong password</t>
         </is>
       </c>
-      <c r="G6" s="2" t="inlineStr">
+      <c r="G6" t="inlineStr">
         <is>
           <t>Error message appears</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="inlineStr">
+      <c r="A7" t="inlineStr">
         <is>
           <t>User Registration</t>
         </is>
       </c>
-      <c r="B7" s="2" t="inlineStr">
+      <c r="B7" t="inlineStr">
         <is>
           <t>TC-003</t>
         </is>
       </c>
-      <c r="C7" s="2" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>Register new user</t>
         </is>
       </c>
-      <c r="D7" s="2" t="inlineStr">
-        <is>
-          <t>Test user registration</t>
-        </is>
-      </c>
-      <c r="E7" s="2" t="n">
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Test user registration with valid information</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
         <v>1</v>
       </c>
-      <c r="F7" s="2" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>Navigate to registration page</t>
         </is>
       </c>
-      <c r="G7" s="2" t="inlineStr">
+      <c r="G7" t="inlineStr">
         <is>
           <t>Registration form is displayed</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="2" t="inlineStr">
+      <c r="A8" t="inlineStr">
         <is>
           <t>User Registration</t>
         </is>
       </c>
-      <c r="B8" s="2" t="inlineStr">
+      <c r="B8" t="inlineStr">
         <is>
           <t>TC-003</t>
         </is>
       </c>
-      <c r="C8" s="2" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>Register new user</t>
         </is>
       </c>
-      <c r="D8" s="2" t="inlineStr">
-        <is>
-          <t>Test user registration</t>
-        </is>
-      </c>
-      <c r="E8" s="2" t="n">
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Test user registration with valid information</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
         <v>2</v>
       </c>
-      <c r="F8" s="2" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>Fill in all required fields</t>
         </is>
       </c>
-      <c r="G8" s="2" t="inlineStr">
+      <c r="G8" t="inlineStr">
         <is>
           <t>Fields are filled correctly</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="2" t="inlineStr">
+      <c r="A9" t="inlineStr">
         <is>
           <t>User Registration</t>
         </is>
       </c>
-      <c r="B9" s="2" t="inlineStr">
+      <c r="B9" t="inlineStr">
         <is>
           <t>TC-003</t>
         </is>
       </c>
-      <c r="C9" s="2" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>Register new user</t>
         </is>
       </c>
-      <c r="D9" s="2" t="inlineStr">
-        <is>
-          <t>Test user registration</t>
-        </is>
-      </c>
-      <c r="E9" s="2" t="n">
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Test user registration with valid information</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
         <v>3</v>
       </c>
-      <c r="F9" s="2" t="inlineStr">
+      <c r="F9" t="inlineStr">
         <is>
           <t>Click Register button</t>
         </is>
       </c>
-      <c r="G9" s="2" t="inlineStr">
+      <c r="G9" t="inlineStr">
         <is>
           <t>Registration successful message appears</t>
         </is>
@@ -802,7 +788,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -810,286 +796,369 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="30" customWidth="1" min="1" max="1"/>
-    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="35" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
     <col width="60" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>Test Case Import Template - Instructions</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="4" t="inlineStr"/>
+      <c r="A2" t="inlineStr"/>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" s="5" t="inlineStr">
+      <c r="A3" s="3" t="inlineStr">
         <is>
           <t>OVERVIEW</t>
         </is>
       </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="inlineStr">
-        <is>
-          <t>This template is used to import test suites, test cases, and test steps into the system.</t>
-        </is>
-      </c>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>This template is used to import submodules, test cases, and test steps into the system.</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" s="4" t="inlineStr"/>
+      <c r="A5" t="inlineStr"/>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" s="5" t="inlineStr">
+      <c r="A6" s="3" t="inlineStr">
         <is>
           <t>COLUMNS</t>
         </is>
       </c>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" s="4" t="inlineStr">
-        <is>
-          <t>Suite Name</t>
-        </is>
-      </c>
-      <c r="B7" s="4" t="inlineStr">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Submodule Name</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
         <is>
           <t>Required</t>
         </is>
       </c>
-      <c r="C7" s="4" t="inlineStr">
-        <is>
-          <t>Name of the test suite. Multiple rows with the same suite name will be grouped together.</t>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Name of the submodule. Multiple rows with the same submodule name will be grouped together.</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="4" t="inlineStr">
+      <c r="A8" t="inlineStr">
         <is>
           <t>Test Case ID</t>
         </is>
       </c>
-      <c r="B8" s="4" t="inlineStr">
+      <c r="B8" t="inlineStr">
         <is>
           <t>Required</t>
         </is>
       </c>
-      <c r="C8" s="4" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>Unique identifier for the test case (e.g., TC-001). Multiple rows with the same ID will be grouped as steps.</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="4" t="inlineStr">
+      <c r="A9" t="inlineStr">
         <is>
           <t>Title</t>
         </is>
       </c>
-      <c r="B9" s="4" t="inlineStr">
+      <c r="B9" t="inlineStr">
         <is>
           <t>Required</t>
         </is>
       </c>
-      <c r="C9" s="4" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>Descriptive title of the test case.</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="4" t="inlineStr">
+      <c r="A10" t="inlineStr">
         <is>
           <t>Description</t>
         </is>
       </c>
-      <c r="B10" s="4" t="inlineStr">
+      <c r="B10" t="inlineStr">
         <is>
           <t>Optional</t>
         </is>
       </c>
-      <c r="C10" s="4" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>Detailed description of what the test case verifies.</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="4" t="inlineStr">
+      <c r="A11" t="inlineStr">
         <is>
           <t>Step Number</t>
         </is>
       </c>
-      <c r="B11" s="4" t="inlineStr">
+      <c r="B11" t="inlineStr">
         <is>
           <t>Required</t>
         </is>
       </c>
-      <c r="C11" s="4" t="inlineStr">
+      <c r="C11" t="inlineStr">
         <is>
           <t>Sequential number for each step (1, 2, 3, ...). Must be sequential within each test case.</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="4" t="inlineStr">
+      <c r="A12" t="inlineStr">
         <is>
           <t>Action</t>
         </is>
       </c>
-      <c r="B12" s="4" t="inlineStr">
+      <c r="B12" t="inlineStr">
         <is>
           <t>Required</t>
         </is>
       </c>
-      <c r="C12" s="4" t="inlineStr">
+      <c r="C12" t="inlineStr">
         <is>
           <t>The action to perform in this step.</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="4" t="inlineStr">
+      <c r="A13" t="inlineStr">
         <is>
           <t>Expected Result</t>
         </is>
       </c>
-      <c r="B13" s="4" t="inlineStr">
+      <c r="B13" t="inlineStr">
         <is>
           <t>Required</t>
         </is>
       </c>
-      <c r="C13" s="4" t="inlineStr">
+      <c r="C13" t="inlineStr">
         <is>
           <t>The expected outcome after performing the action.</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="4" t="inlineStr"/>
+      <c r="A14" t="inlineStr"/>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr"/>
     </row>
     <row r="15">
-      <c r="A15" s="5" t="inlineStr">
+      <c r="A15" s="3" t="inlineStr">
         <is>
           <t>RULES</t>
         </is>
       </c>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr"/>
     </row>
     <row r="16">
-      <c r="A16" s="4" t="inlineStr">
+      <c r="A16" t="inlineStr">
         <is>
           <t>• All required fields must be filled.</t>
         </is>
       </c>
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" t="inlineStr"/>
     </row>
     <row r="17">
-      <c r="A17" s="4" t="inlineStr">
-        <is>
-          <t>• Suite Name must be the same for all test cases in the same suite.</t>
-        </is>
-      </c>
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>• Submodule Name must be the same for all test cases in the same submodule.</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr"/>
+      <c r="C17" t="inlineStr"/>
     </row>
     <row r="18">
-      <c r="A18" s="4" t="inlineStr">
+      <c r="A18" t="inlineStr">
         <is>
           <t>• Test Case ID must be the same for all steps in the same test case.</t>
         </is>
       </c>
+      <c r="B18" t="inlineStr"/>
+      <c r="C18" t="inlineStr"/>
     </row>
     <row r="19">
-      <c r="A19" s="4" t="inlineStr">
+      <c r="A19" t="inlineStr">
         <is>
           <t>• Step Number must be sequential (1, 2, 3, ...) within each test case.</t>
         </is>
       </c>
+      <c r="B19" t="inlineStr"/>
+      <c r="C19" t="inlineStr"/>
     </row>
     <row r="20">
-      <c r="A20" s="4" t="inlineStr">
+      <c r="A20" t="inlineStr">
         <is>
           <t>• Test Case ID must be unique within the module (duplicates will be skipped).</t>
         </is>
       </c>
+      <c r="B20" t="inlineStr"/>
+      <c r="C20" t="inlineStr"/>
     </row>
     <row r="21">
-      <c r="A21" s="4" t="inlineStr">
+      <c r="A21" s="3" t="inlineStr">
         <is>
           <t>• Delete sample data rows before adding your own data.</t>
         </is>
       </c>
+      <c r="B21" t="inlineStr"/>
+      <c r="C21" t="inlineStr"/>
     </row>
     <row r="22">
-      <c r="A22" s="4" t="inlineStr"/>
+      <c r="A22" t="inlineStr"/>
+      <c r="B22" t="inlineStr"/>
+      <c r="C22" t="inlineStr"/>
     </row>
     <row r="23">
-      <c r="A23" s="5" t="inlineStr">
+      <c r="A23" t="inlineStr">
         <is>
           <t>EXAMPLE</t>
         </is>
       </c>
+      <c r="B23" t="inlineStr"/>
+      <c r="C23" t="inlineStr"/>
     </row>
     <row r="24">
-      <c r="A24" s="4" t="inlineStr">
+      <c r="A24" t="inlineStr">
         <is>
           <t>To create a test case with 3 steps:</t>
         </is>
       </c>
+      <c r="B24" t="inlineStr"/>
+      <c r="C24" t="inlineStr"/>
     </row>
     <row r="25">
-      <c r="A25" s="4" t="inlineStr">
-        <is>
-          <t>1. Enter the same Suite Name for all 3 rows</t>
-        </is>
-      </c>
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>1. Enter the same Submodule Name for all 3 rows</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr"/>
+      <c r="C25" t="inlineStr"/>
     </row>
     <row r="26">
-      <c r="A26" s="4" t="inlineStr">
+      <c r="A26" t="inlineStr">
         <is>
           <t>2. Enter the same Test Case ID for all 3 rows</t>
         </is>
       </c>
+      <c r="B26" t="inlineStr"/>
+      <c r="C26" t="inlineStr"/>
     </row>
     <row r="27">
-      <c r="A27" s="4" t="inlineStr">
+      <c r="A27" s="3" t="inlineStr">
         <is>
           <t>3. Enter the same Title for all 3 rows</t>
         </is>
       </c>
+      <c r="B27" t="inlineStr"/>
+      <c r="C27" t="inlineStr"/>
     </row>
     <row r="28">
-      <c r="A28" s="4" t="inlineStr">
+      <c r="A28" t="inlineStr">
         <is>
           <t>4. Enter Step Number 1, 2, and 3 respectively</t>
         </is>
       </c>
+      <c r="B28" t="inlineStr"/>
+      <c r="C28" t="inlineStr"/>
     </row>
     <row r="29">
-      <c r="A29" s="4" t="inlineStr">
+      <c r="A29" t="inlineStr">
         <is>
           <t>5. Enter different Actions and Expected Results for each step</t>
         </is>
       </c>
+      <c r="B29" t="inlineStr"/>
+      <c r="C29" t="inlineStr"/>
     </row>
     <row r="30">
-      <c r="A30" s="4" t="inlineStr"/>
+      <c r="A30" t="inlineStr"/>
+      <c r="B30" t="inlineStr"/>
+      <c r="C30" t="inlineStr"/>
     </row>
     <row r="31">
-      <c r="A31" s="4" t="inlineStr">
+      <c r="A31" s="3" t="inlineStr">
+        <is>
+          <t>GROUPING PATTERN</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr"/>
+      <c r="C31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Multiple test cases can be in the same submodule by using the same Submodule Name.</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr"/>
+      <c r="C32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Multiple test steps can be in the same test case by using the same Test Case ID.</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr"/>
+      <c r="C33" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr"/>
+      <c r="B34" t="inlineStr"/>
+      <c r="C34" t="inlineStr"/>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
         <is>
           <t>SUPPORT</t>
         </is>
       </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="4" t="inlineStr">
+      <c r="B35" t="inlineStr"/>
+      <c r="C35" t="inlineStr"/>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
         <is>
           <t>For issues or questions, contact your system administrator.</t>
         </is>
       </c>
+      <c r="B36" t="inlineStr"/>
+      <c r="C36" t="inlineStr"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>